<commit_message>
change settings to match Arduino based firmware
</commit_message>
<xml_diff>
--- a/docs/RAMPS连接说明.xlsx
+++ b/docs/RAMPS连接说明.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="7020" yWindow="5020" windowWidth="28800" windowHeight="16440" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16560" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="工作表1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="42">
   <si>
     <t>RAMPS连接说明</t>
     <rPh sb="5" eb="6">
@@ -108,16 +108,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>挤出头(并联臂)</t>
-    <rPh sb="0" eb="1">
-      <t>ji'c't</t>
-    </rPh>
-    <rPh sb="4" eb="5">
-      <t>b'l'bi</t>
-    </rPh>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>挤出头</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -179,10 +169,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>T0</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>挤出头热电阻</t>
     <rPh sb="0" eb="1">
       <t>j'c't</t>
@@ -190,10 +176,6 @@
     <rPh sb="3" eb="4">
       <t>re'd'z</t>
     </rPh>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>T1</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -208,40 +190,61 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
+    <t>调试</t>
+    <rPh sb="0" eb="1">
+      <t>tia's</t>
+    </rPh>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>UART1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>SWD</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>AUX-1(A3-CLK,A4-IO)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>AUX-1(TxD,RxD)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>T1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>组件</t>
-    <rPh sb="0" eb="1">
-      <t>zu'j</t>
-    </rPh>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>接口</t>
-    <rPh sb="0" eb="1">
-      <t>jie'kou</t>
-    </rPh>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>调试</t>
-    <rPh sb="0" eb="1">
-      <t>tia's</t>
-    </rPh>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>UART1</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>SWD</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>AUX-1(A3-CLK,A4-IO)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>AUX-1(TxD,RxD)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>并联臂</t>
+    <rPh sb="0" eb="1">
+      <t>bin'l'b</t>
+    </rPh>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>串联臂</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Y-max</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Z-max</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Z-min</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -249,7 +252,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -262,6 +265,32 @@
       <sz val="9"/>
       <name val="宋体"/>
       <family val="2"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
+      <name val="宋体"/>
+      <family val="2"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="11"/>
+      <name val="宋体"/>
+      <family val="2"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="宋体"/>
+      <family val="3"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
@@ -283,17 +312,26 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="5">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
+    <cellStyle name="超链接" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="4" builtinId="9" hidden="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium7"/>
@@ -649,35 +687,45 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C19"/>
+  <dimension ref="A1:D19"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="A22" sqref="A22"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C27" sqref="C27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="13.6640625" customWidth="1"/>
     <col min="2" max="2" width="17.5" customWidth="1"/>
-    <col min="3" max="3" width="30.5" customWidth="1"/>
+    <col min="3" max="3" width="22" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="B3" t="s">
-        <v>32</v>
-      </c>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A2" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B2" s="1"/>
+      <c r="C2" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="D2" s="1"/>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.15">
       <c r="C3" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.15">
+        <v>37</v>
+      </c>
+      <c r="D3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A4" t="s">
         <v>1</v>
       </c>
@@ -688,7 +736,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.15">
       <c r="B5" t="s">
         <v>4</v>
       </c>
@@ -696,7 +744,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.15">
       <c r="B6" t="s">
         <v>6</v>
       </c>
@@ -704,15 +752,15 @@
         <v>7</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.15">
       <c r="B7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C7" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A8" t="s">
         <v>8</v>
       </c>
@@ -720,109 +768,120 @@
         <v>10</v>
       </c>
       <c r="C8" t="s">
+        <v>17</v>
+      </c>
+      <c r="D8" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.15">
       <c r="B9" t="s">
         <v>12</v>
       </c>
       <c r="C9" t="s">
+        <v>39</v>
+      </c>
+      <c r="D9" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.15">
       <c r="B10" t="s">
         <v>7</v>
       </c>
       <c r="C10" t="s">
+        <v>40</v>
+      </c>
+      <c r="D10" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.15">
       <c r="B11" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C11" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A12" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A12" t="s">
+      <c r="B12" t="s">
         <v>19</v>
       </c>
-      <c r="B12" t="s">
+      <c r="C12" t="s">
         <v>20</v>
       </c>
-      <c r="C12" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.15">
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.15">
       <c r="B13" t="s">
         <v>15</v>
       </c>
       <c r="C13" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="B14" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="B14" t="s">
+      <c r="C14" t="s">
         <v>23</v>
       </c>
-      <c r="C14" t="s">
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A15" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A15" t="s">
+      <c r="B15" t="s">
         <v>25</v>
       </c>
-      <c r="B15" t="s">
+      <c r="C15" s="2" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="B16" t="s">
         <v>26</v>
       </c>
-      <c r="C15" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="B16" t="s">
-        <v>28</v>
-      </c>
       <c r="C16" t="s">
-        <v>29</v>
+        <v>9</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.15">
       <c r="B17" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="C17" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A18" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="B18" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="C18" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.15">
       <c r="B19" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="C19" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="1">
+  <mergeCells count="3">
     <mergeCell ref="A1:C1"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="C2:D2"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>